<commit_message>
Added plot function to plot stacked end-uses
</commit_message>
<xml_diff>
--- a/data/residential_model/_EXCELFILES/SANSOM_residential_gas_hourly_shape.xlsx
+++ b/data/residential_model/_EXCELFILES/SANSOM_residential_gas_hourly_shape.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Day</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>in %</t>
+  </si>
+  <si>
+    <t>PEAK</t>
+  </si>
+  <si>
+    <t>PEAK READ FROM CHART</t>
+  </si>
+  <si>
+    <t>absolute</t>
+  </si>
+  <si>
+    <t>percent</t>
   </si>
 </sst>
 </file>
@@ -100,14 +112,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -117,7 +129,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11677650" y="4429125"/>
+          <a:off x="11620500" y="5191125"/>
           <a:ext cx="3962400" cy="4762500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -187,6 +199,61 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>179205</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4219575" y="5248275"/>
+          <a:ext cx="11668125" cy="7122930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -479,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,6 +857,83 @@
       </c>
       <c r="Y4">
         <v>1.9285886137947834</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.54884742041712398</v>
+      </c>
+      <c r="C5">
+        <v>0.54884742041712398</v>
+      </c>
+      <c r="D5">
+        <v>0.54884742041712398</v>
+      </c>
+      <c r="E5">
+        <v>0.54884742041712398</v>
+      </c>
+      <c r="F5">
+        <v>0.65861690450054877</v>
+      </c>
+      <c r="G5">
+        <v>2.1953896816684959</v>
+      </c>
+      <c r="H5">
+        <v>4.6103183315038416</v>
+      </c>
+      <c r="I5">
+        <v>6.5861690450054873</v>
+      </c>
+      <c r="J5">
+        <v>9.6597145993413829</v>
+      </c>
+      <c r="K5">
+        <v>3.2930845225027436</v>
+      </c>
+      <c r="L5">
+        <v>5.0493962678375404</v>
+      </c>
+      <c r="M5">
+        <v>5.48847420417124</v>
+      </c>
+      <c r="N5">
+        <v>4.171240395170142</v>
+      </c>
+      <c r="O5">
+        <v>4.3907793633369918</v>
+      </c>
+      <c r="P5">
+        <v>4.6103183315038416</v>
+      </c>
+      <c r="Q5">
+        <v>5.1591657519209653</v>
+      </c>
+      <c r="R5">
+        <v>4.7200878155872656</v>
+      </c>
+      <c r="S5">
+        <v>7.2447859495060358</v>
+      </c>
+      <c r="T5">
+        <v>7.4643249176728856</v>
+      </c>
+      <c r="U5">
+        <v>7.1350164654226118</v>
+      </c>
+      <c r="V5">
+        <v>6.4763995609220633</v>
+      </c>
+      <c r="W5">
+        <v>5.48847420417124</v>
+      </c>
+      <c r="X5">
+        <v>2.1953896816684959</v>
+      </c>
+      <c r="Y5">
+        <v>1.2074643249176729</v>
       </c>
     </row>
   </sheetData>
@@ -799,10 +943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW18"/>
+  <dimension ref="A1:AW24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:Y18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,7 +2137,7 @@
         <v>0.77780676961992012</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:Z17" si="26">(100/$Z10)*C10</f>
+        <f t="shared" ref="C17:Y17" si="26">(100/$Z10)*C10</f>
         <v>0.56979892645607844</v>
       </c>
       <c r="D17">
@@ -2098,7 +2242,7 @@
         <v>0.90445503450092357</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:Z18" si="27">(100/$Z11)*C11</f>
+        <f t="shared" ref="C18:Y18" si="27">(100/$Z11)*C11</f>
         <v>0.70351423989588246</v>
       </c>
       <c r="D18">
@@ -2191,6 +2335,271 @@
       </c>
       <c r="Z18">
         <f>SUM(B18:Y18)</f>
+        <v>99.999999999999972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <v>8</v>
+      </c>
+      <c r="K22">
+        <v>9</v>
+      </c>
+      <c r="L22">
+        <v>10</v>
+      </c>
+      <c r="M22">
+        <v>11</v>
+      </c>
+      <c r="N22">
+        <v>12</v>
+      </c>
+      <c r="O22">
+        <v>13</v>
+      </c>
+      <c r="P22">
+        <v>14</v>
+      </c>
+      <c r="Q22">
+        <v>15</v>
+      </c>
+      <c r="R22">
+        <v>16</v>
+      </c>
+      <c r="S22">
+        <v>17</v>
+      </c>
+      <c r="T22">
+        <v>18</v>
+      </c>
+      <c r="U22">
+        <v>19</v>
+      </c>
+      <c r="V22">
+        <v>20</v>
+      </c>
+      <c r="W22">
+        <v>21</v>
+      </c>
+      <c r="X22">
+        <v>22</v>
+      </c>
+      <c r="Y22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>0.5</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>0.5</v>
+      </c>
+      <c r="E23">
+        <v>0.5</v>
+      </c>
+      <c r="F23">
+        <v>0.6</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>4.2</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+      <c r="N23">
+        <v>3.8</v>
+      </c>
+      <c r="O23">
+        <v>4</v>
+      </c>
+      <c r="P23">
+        <v>4.2</v>
+      </c>
+      <c r="Q23">
+        <v>4.7</v>
+      </c>
+      <c r="R23">
+        <v>4.3</v>
+      </c>
+      <c r="S23">
+        <v>6.6</v>
+      </c>
+      <c r="T23">
+        <v>6.8</v>
+      </c>
+      <c r="U23">
+        <v>6.5</v>
+      </c>
+      <c r="V23">
+        <v>5.9</v>
+      </c>
+      <c r="W23">
+        <v>5</v>
+      </c>
+      <c r="X23">
+        <v>2</v>
+      </c>
+      <c r="Y23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z23">
+        <f>SUM(B23:Y23)</f>
+        <v>91.100000000000009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <f>100/$Z$23*B23</f>
+        <v>0.54884742041712398</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:Y24" si="28">100/$Z$23*C23</f>
+        <v>0.54884742041712398</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="28"/>
+        <v>0.54884742041712398</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="28"/>
+        <v>0.54884742041712398</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="28"/>
+        <v>0.65861690450054877</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="28"/>
+        <v>2.1953896816684959</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="28"/>
+        <v>4.6103183315038416</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="28"/>
+        <v>6.5861690450054873</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="28"/>
+        <v>9.6597145993413829</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="28"/>
+        <v>3.2930845225027436</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="28"/>
+        <v>5.0493962678375404</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="28"/>
+        <v>5.48847420417124</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="28"/>
+        <v>4.171240395170142</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="28"/>
+        <v>4.3907793633369918</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="28"/>
+        <v>4.6103183315038416</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="28"/>
+        <v>5.1591657519209653</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="28"/>
+        <v>4.7200878155872656</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="28"/>
+        <v>7.2447859495060358</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="28"/>
+        <v>7.4643249176728856</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="28"/>
+        <v>7.1350164654226118</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="28"/>
+        <v>6.4763995609220633</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="28"/>
+        <v>5.48847420417124</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="28"/>
+        <v>2.1953896816684959</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="28"/>
+        <v>1.2074643249176729</v>
+      </c>
+      <c r="Z24">
+        <f>SUM(B24:Y24)</f>
         <v>99.999999999999972</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Can drow load factors. Still however strange...
</commit_message>
<xml_diff>
--- a/data/residential_model/_EXCELFILES/SANSOM_residential_gas_hourly_shape.xlsx
+++ b/data/residential_model/_EXCELFILES/SANSOM_residential_gas_hourly_shape.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="12315"/>
+    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="12315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -119,97 +119,8 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>original!$B$9:$Y$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.2999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.7</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.9</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -298,87 +209,87 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>original!$B$18:$Y$18</c:f>
+              <c:f>original!$B$11:$Y$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.41580041580041577</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41580041580041577</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41580041580041577</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41580041580041577</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41580041580041577</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2474012474012472</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0790020790020787</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.1975051975051967</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3555093555093549</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.1975051975051967</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.118503118503118</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.3264033264033261</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.1580041580041573</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.3264033264033261</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.3264033264033261</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.365904365904365</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.3160083160083147</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.979209979209978</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.7713097713097703</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.6923076923076916</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.4449064449064437</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.0291060291060283</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.9501039501039492</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.0395010395010393</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,87 +298,87 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>original!$B$24:$Y$24</c:f>
+              <c:f>original!$B$23:$Y$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.56561085972850678</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56561085972850678</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56561085972850678</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56561085972850678</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0361990950226243</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3755656108597285</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.751131221719457</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.7873303167420813</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.4298642533936645</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.3936651583710407</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2036199095022617</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.6561085972850673</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.2986425339366514</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.5248868778280542</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.751131221719457</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.3167420814479636</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.864253393665158</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.4660633484162888</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.6923076923076916</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.3529411764705879</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.6742081447963804</c:v>
+                  <c:v>5.9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.6561085972850673</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2624434389140271</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.244343891402715</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,11 +395,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95673344"/>
-        <c:axId val="95694208"/>
+        <c:axId val="84017536"/>
+        <c:axId val="84019072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95673344"/>
+        <c:axId val="84017536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95694208"/>
+        <c:crossAx val="84019072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -505,7 +416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95694208"/>
+        <c:axId val="84019072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,13 +427,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95673344"/>
+        <c:crossAx val="84017536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1077,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AW24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:Y24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>